<commit_message>
Started presentation, formatted new demographics table w/ correct stratification
</commit_message>
<xml_diff>
--- a/Project1/Reports/DemographicsTable09242017_formatted.xlsx
+++ b/Project1/Reports/DemographicsTable09242017_formatted.xlsx
@@ -19,7 +19,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Hard drugs = Yes</t>
+  </si>
+  <si>
+    <t>Hard drugs = No</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
   <si>
     <t>Age at baseline</t>
   </si>
@@ -27,25 +39,22 @@
     <t>43.27 ± 8.78</t>
   </si>
   <si>
+    <t>44.62 ± 9.49</t>
+  </si>
+  <si>
+    <t>43.16 ± 8.72</t>
+  </si>
+  <si>
     <t>BMI at baseline</t>
   </si>
   <si>
     <t>25.26 ± 4.41</t>
   </si>
   <si>
-    <t>Hard drug use at baseline</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>467 (92.29)</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>39 (7.71)</t>
+    <t>23.62 ± 3.45</t>
+  </si>
+  <si>
+    <t>25.39 ± 4.46</t>
   </si>
   <si>
     <t>Alcohol use at baseline</t>
@@ -57,27 +66,54 @@
     <t>471 (93.08)</t>
   </si>
   <si>
+    <t>37 (94.87)</t>
+  </si>
+  <si>
+    <t>434 (92.93)</t>
+  </si>
+  <si>
     <t>&gt; 13 drinks per week</t>
   </si>
   <si>
     <t>35 (6.92)</t>
   </si>
   <si>
+    <t>2 (5.13)</t>
+  </si>
+  <si>
+    <t>33 (7.07)</t>
+  </si>
+  <si>
     <t>Smoking status at baseline</t>
   </si>
   <si>
+    <t>&lt;0.0001</t>
+  </si>
+  <si>
     <t>Never/former</t>
   </si>
   <si>
     <t>310 (61.26)</t>
   </si>
   <si>
+    <t>9 (23.08)</t>
+  </si>
+  <si>
+    <t>301 (64.45)</t>
+  </si>
+  <si>
     <t>Current</t>
   </si>
   <si>
     <t>196 (38.74)</t>
   </si>
   <si>
+    <t>30 (76.92)</t>
+  </si>
+  <si>
+    <t>166 (35.55)</t>
+  </si>
+  <si>
     <t>Income level at baseline</t>
   </si>
   <si>
@@ -87,18 +123,33 @@
     <t>105 (20.75)</t>
   </si>
   <si>
+    <t>14 (35.9)</t>
+  </si>
+  <si>
+    <t>91 (20.22)</t>
+  </si>
+  <si>
     <t>$10,000 - $40,000</t>
   </si>
   <si>
     <t>210 (41.5)</t>
   </si>
   <si>
+    <t>16 (41.03)</t>
+  </si>
+  <si>
+    <t>194 (43.11)</t>
+  </si>
+  <si>
     <t>&gt; $40,000</t>
   </si>
   <si>
     <t>174 (34.39)</t>
   </si>
   <si>
+    <t>165 (36.67)</t>
+  </si>
+  <si>
     <t>Education at baseline</t>
   </si>
   <si>
@@ -108,12 +159,21 @@
     <t>111 (21.94)</t>
   </si>
   <si>
+    <t>95 (20.34)</t>
+  </si>
+  <si>
     <t>&gt;HS</t>
   </si>
   <si>
     <t>395 (78.06)</t>
   </si>
   <si>
+    <t>23 (58.97)</t>
+  </si>
+  <si>
+    <t>372 (79.66)</t>
+  </si>
+  <si>
     <t>Adherence at 2 years</t>
   </si>
   <si>
@@ -123,34 +183,70 @@
     <t>52 (10.28)</t>
   </si>
   <si>
+    <t>1 (2.56)</t>
+  </si>
+  <si>
+    <t>51 (10.92)</t>
+  </si>
+  <si>
     <t>&gt;95%</t>
   </si>
   <si>
     <t>454 (89.72)</t>
   </si>
   <si>
+    <t>38 (97.44)</t>
+  </si>
+  <si>
+    <t>416 (89.08)</t>
+  </si>
+  <si>
     <t>Baseline viral load</t>
   </si>
   <si>
     <t>1008772.37 ± 11435068.78</t>
   </si>
   <si>
+    <t>184278.01 ± 430227.28</t>
+  </si>
+  <si>
+    <t>1080547.55 ± 11920119.51</t>
+  </si>
+  <si>
     <t>Baseline CD4+ count</t>
   </si>
   <si>
     <t>374.7 ± 199.7</t>
   </si>
   <si>
-    <t>Baseline AGG_MENT score</t>
+    <t>352.18 ± 194.67</t>
+  </si>
+  <si>
+    <t>376.66 ± 200.22</t>
+  </si>
+  <si>
+    <t>Baseline SF36 MCS score</t>
   </si>
   <si>
     <t>45.23 ± 13.49</t>
   </si>
   <si>
+    <t>42.31 ± 11.22</t>
+  </si>
+  <si>
+    <t>45.48 ± 13.65</t>
+  </si>
+  <si>
+    <t>Baseline SF36 PCS score</t>
+  </si>
+  <si>
     <t>51.03 ± 9.11</t>
   </si>
   <si>
-    <t>Baseline AGG_PHYS score</t>
+    <t>47.7 ± 8.5</t>
+  </si>
+  <si>
+    <t>51.31 ± 9.11</t>
   </si>
 </sst>
 </file>
@@ -493,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -608,6 +704,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -653,23 +802,56 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -992,201 +1174,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6"/>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+    <row r="2" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="B2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C2" s="18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="D2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="E2" s="18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="E3" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="D5" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+    <row r="6" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B6" s="17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="C6" s="18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+      <c r="D6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="8" t="s">
+    </row>
+    <row r="8" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="B8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C8" s="18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="D8" s="19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B9" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="D9" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+    <row r="10" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="7"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="18">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B11" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="D11" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+    <row r="12" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B12" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="C12" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="D12" s="19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B13" s="11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>42</v>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.16300000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="18">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.45600000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="18">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>